<commit_message>
added new stimfile for round3
</commit_message>
<xml_diff>
--- a/stim_folder/stimuli_round3.xlsx
+++ b/stim_folder/stimuli_round3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amsuni-my.sharepoint.com/personal/a_palmann_uva_nl/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amsuni-my.sharepoint.com/personal/a_palmann_uva_nl/Documents/Microsoft Teams Chat Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{F544EB10-FB11-44B7-AA8E-13784B7427AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50ADB449-12B4-4BF1-BBA9-A6F191B272FA}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{F544EB10-FB11-44B7-AA8E-13784B7427AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B95F138F-98EE-4B5C-9BEF-C9A15F666DDC}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5C6A6CE9-FAAA-4323-9214-A09E4F61C974}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="96">
   <si>
     <t>m_1 Willi Baumeister - Aru mit Gelb.tif</t>
   </si>
@@ -53,12 +53,6 @@
     <t>mirror</t>
   </si>
   <si>
-    <t>img_22</t>
-  </si>
-  <si>
-    <t>Het schilderij toont een sterk contrast van zwarte en gele vormen, met extra accenten van rood, wit en groen. De vormen zijn onregelmatig en krachtig, en lijken gefragmenteerde stukken die een dynamische interactie creëren. Het gele gedeelte domineert, met getextureerde randen die het contrast verzachten.</t>
-  </si>
-  <si>
     <t>De Kooning 165 Untitled II.tif</t>
   </si>
   <si>
@@ -74,15 +68,6 @@
     <t>match2</t>
   </si>
   <si>
-    <t>img_8</t>
-  </si>
-  <si>
-    <t>Het schilderij toont gedurfde en chaotische penseelstreken in rood, groen, wit en geel. De kleuren mengen zich dynamisch, wat een gevoel van energie en intensiteit geeft.</t>
-  </si>
-  <si>
-    <t>very short</t>
-  </si>
-  <si>
     <t>Klee 328 Haus_ aussen und innen.tif</t>
   </si>
   <si>
@@ -95,12 +80,6 @@
     <t>Klee 321 Farbtafel (auf maiorem Grau).tif</t>
   </si>
   <si>
-    <t>img_17</t>
-  </si>
-  <si>
-    <t>Het schilderij toont een raster van vierkanten en rechthoeken die concentrisch zijn gerangschikt, met een verloop van lichtroze in het midden naar donkerbruin en zwart aan de randen. De kleurovergang is vloeiend, wat een gloedachtig effect creëert. De randen zijn zacht geblend, wat de compositie een harmonieuze en samenhangende uitstraling geeft.</t>
-  </si>
-  <si>
     <t>Kljun-MM-06.tif</t>
   </si>
   <si>
@@ -113,12 +92,6 @@
     <t>Mondrian-PM-07.tif</t>
   </si>
   <si>
-    <t>img_18</t>
-  </si>
-  <si>
-    <t>Het schilderij toont geometrische vormen zoals rechthoeken en lijnen in kleuren zoals zwart, oranje, rood en groen. De vormen lijken gelaagd en schuin geplaatst tegen een witte achtergrond. Fijne lijnen en bogen kruisen de compositie en geven een gevoel van beweging.</t>
-  </si>
-  <si>
     <t>Louis-AP-08.tif</t>
   </si>
   <si>
@@ -131,15 +104,6 @@
     <t>m_Motherwell 77 Medusa Series.tif</t>
   </si>
   <si>
-    <t>img_26</t>
-  </si>
-  <si>
-    <t>Een compositie van horizontale, langwerpige vormen in verschillende kleuren, waaronder bruin, groen, geel en rood. De vormen hebben zachte randen en vloeien naadloos in elkaar over. De achtergrond is neutraal beige, wat het contrast van de gekleurde vormen benadrukt.</t>
-  </si>
-  <si>
-    <t>does not start with het schilderij, short</t>
-  </si>
-  <si>
     <t>2 Olga Rosanowa - Ungegenstaendliche Komposition.tif</t>
   </si>
   <si>
@@ -152,12 +116,6 @@
     <t>m_Moholy Nagy 28 Komposition Q XX.tif</t>
   </si>
   <si>
-    <t>img_6</t>
-  </si>
-  <si>
-    <t>Het schilderij toont twee grote rode rechthoeken die verticaal gestapeld zijn, gescheiden door een dikke zwarte horizontale lijn. De achtergrond is een gedempte gele kleur die de compositie omlijst.</t>
-  </si>
-  <si>
     <t>Hofmann (keine Seite; Nr.2) House in Storm.tif</t>
   </si>
   <si>
@@ -170,15 +128,6 @@
     <t>m_Hofmann (keine Seite; Nr.2) House in Storm.tif</t>
   </si>
   <si>
-    <t>img_25</t>
-  </si>
-  <si>
-    <t>Een levendige compositie van draaiende, overlappende penseelstreken. Overheerst door rood, geel en groen met accenten van blauw. De dikke verfaanbreng creëert een textuur en dynamisch oppervlak. De vormen zijn vaag, maar suggereren beweging en energie.</t>
-  </si>
-  <si>
-    <t>does not start with het schilderij</t>
-  </si>
-  <si>
     <t>Hoehme-AP-24.tif</t>
   </si>
   <si>
@@ -194,15 +143,6 @@
     <t>match4</t>
   </si>
   <si>
-    <t>img_15</t>
-  </si>
-  <si>
-    <t>Het schilderij toont een getextureerd oppervlak gevuld met talloze ingekerfde lijnen, symbolen en geometrische vormen. De achtergrond is een mix van aardse, vervaagde tinten, wat een rustieke en verouderde uitstraling geeft. Het oppervlak lijkt op een bekrast of ingeschreven muur, vol details en visuele drukte.</t>
-  </si>
-  <si>
-    <t>short</t>
-  </si>
-  <si>
     <t>Mondrian-PM-08.tif</t>
   </si>
   <si>
@@ -215,12 +155,6 @@
     <t>Twombly-AP-17.tif</t>
   </si>
   <si>
-    <t>img_30</t>
-  </si>
-  <si>
-    <t>Het schilderij bestaat uit een raster van zwarte lijnen die rechthoeken en vierkanten vormen, gevuld met primaire kleuren (rood, blauw, geel) en neutrale tinten (wit, grijs en zwart). De compositie is geometrisch, zonder gebogen vormen, met nadruk op rechte lijnen en hoeken.</t>
-  </si>
-  <si>
     <t>Nay 133 - Gelb.tif</t>
   </si>
   <si>
@@ -233,9 +167,6 @@
     <t>Reinhardt-PA-28.tif</t>
   </si>
   <si>
-    <t>img_31</t>
-  </si>
-  <si>
     <t>Nay-AP-10.tif</t>
   </si>
   <si>
@@ -248,12 +179,6 @@
     <t>Francis-AP-18.tif</t>
   </si>
   <si>
-    <t>img_32</t>
-  </si>
-  <si>
-    <t>Het schilderij toont een verzameling abstracte vormen in levendige rood-, blauw-, geel- en zwarttinten, tegen een beige achtergrond met textuur. Zwarte lijnen kruisen en buigen dynamisch over het doek, wat energie en contrast toevoegt.</t>
-  </si>
-  <si>
     <t>Nay-BJ-32.tif</t>
   </si>
   <si>
@@ -266,12 +191,6 @@
     <t>Richter 218 Abstract Painting.tif</t>
   </si>
   <si>
-    <t>img_33</t>
-  </si>
-  <si>
-    <t>Een dynamische abstracte compositie met opvallende gele, blauwe, zwarte en witte kleuren. Krullende vormen domineren, waardoor een gevoel van beweging en gelaagde diepte ontstaat. Sommige penseelstreken zijn dik en doelbewust, terwijl andere vloeiender en losser lijken.</t>
-  </si>
-  <si>
     <t>Pollock-JP-06.tif</t>
   </si>
   <si>
@@ -284,15 +203,6 @@
     <t>3 Philip Guston - For M.tif</t>
   </si>
   <si>
-    <t>img_34</t>
-  </si>
-  <si>
-    <t>Een ingewikkeld netwerk van gespatte en druipende verf in zwart, geel, blauw en rood. De textuur lijkt chaotisch maar beheerst, met overlappende lagen verf die een dicht en levendig oppervlak creëren.</t>
-  </si>
-  <si>
-    <t>does not start with het schilderij, very short</t>
-  </si>
-  <si>
     <t>Pollock-PA-01.tif</t>
   </si>
   <si>
@@ -305,12 +215,6 @@
     <t>Pollock-PA-05.tif</t>
   </si>
   <si>
-    <t>img_35</t>
-  </si>
-  <si>
-    <t>Een complexe mix van draaiende en hoekige witte, blauwe, rode en bruine streken op een lichtere achtergrond. Figuren en vormen lijken tevoorschijn te komen en op te gaan in de energieke lijnen en lagen.</t>
-  </si>
-  <si>
     <t>Francis-PA-14.tif</t>
   </si>
   <si>
@@ -323,12 +227,6 @@
     <t>m_Kline-PA-20.tif</t>
   </si>
   <si>
-    <t>img_24</t>
-  </si>
-  <si>
-    <t>Een wit canvas met verspreide abstracte verfvlekken. De streken zijn dun, gestippeld en golvend, voornamelijk in blauw, geel en rood. Verfspatten strekken zich uit over het oppervlak, wat een gevoel van beweging creëert. De randen van het schilderij hebben geconcentreerde kleurvlakken, terwijl het midden relatief leeg blijft.</t>
-  </si>
-  <si>
     <t>3 Richard Diebenkorn - Urbana No. 6.Seite 66.tif</t>
   </si>
   <si>
@@ -341,12 +239,6 @@
     <t>3 Joan Mitchell - Hemlock.tif</t>
   </si>
   <si>
-    <t>img_7</t>
-  </si>
-  <si>
-    <t>Het schilderij is een complexe abstracte compositie met verspreide zwarte, witte en pastelkleuren. Het bevat overlappende lijnen en vormen, wat een gevoel van beweging en fragmentatie oproept.</t>
-  </si>
-  <si>
     <t>Rothko-RR-08.tif</t>
   </si>
   <si>
@@ -359,12 +251,6 @@
     <t>Rothko-RR-04.tif</t>
   </si>
   <si>
-    <t>img_38</t>
-  </si>
-  <si>
-    <t>Het schilderij bestaat uit zachte, rechthoekige vormen in gedempte kleuren zoals oranje, blauw, beige en groenachtig grijs. De randen van de vormen zijn vaag en vloeien in elkaar en de achtergrond over. De compositie is eenvoudig maar gelaagd, met een rustige, sfeervolle uitstraling. Het geheel oogt zacht en diffuus.</t>
-  </si>
-  <si>
     <t>Smith-PA-30.tif</t>
   </si>
   <si>
@@ -377,12 +263,6 @@
     <t>2 Wols - ohne Titel (Baeume).tif</t>
   </si>
   <si>
-    <t>img_39</t>
-  </si>
-  <si>
-    <t>Het schilderij bestaat uit stevige zwarte penseelstreken verspreid over een lichte achtergrond. De streken zijn onregelmatig, overlappen elkaar en variëren in dikte. Sommige streken lijken op organische vormen, terwijl andere meer lineair zijn. De compositie voelt dynamisch en energiek aan, zonder een specifiek focuspunt. Bovenaan is een zwakke handtekening zichtbaar, mogelijk van de kunstenaar, met een datum.</t>
-  </si>
-  <si>
     <t>Mondrian-PM-03.tif</t>
   </si>
   <si>
@@ -395,15 +275,6 @@
     <t>Pollock-JP-01.tif</t>
   </si>
   <si>
-    <t>img_29</t>
-  </si>
-  <si>
-    <t>Het schilderij is een compositie van rechthoeken en vierkanten in verschillende tinten geel, grijs en beige, omlijnd met zwart. De vormen zijn gerangschikt in een onregelmatig, rasterachtig patroon met overlappende elementen. Sommige gebieden hebben subtiele schaduwen, wat diepte toevoegt. Rechtsonder staat de naam van de kunstenaar "Mondrian."</t>
-  </si>
-  <si>
-    <t>name of artist mentioned</t>
-  </si>
-  <si>
     <t>2 Barnett Newman - White fire I.tif</t>
   </si>
   <si>
@@ -416,12 +287,6 @@
     <t>Hesse 104 64. Sans titre (Two Circles).tif</t>
   </si>
   <si>
-    <t>img_41</t>
-  </si>
-  <si>
-    <t>Het schilderij toont twee verticale lijnen op een lichtgekleurde achtergrond. Eén lijn is beige en heeft strakke randen, terwijl de andere donkerblauw is met ruwe, textuurachtige randen. De lijnen staan van elkaar af, waardoor een minimalistische compositie ontstaat met veel negatieve ruimte. Rechtsonder is een kleine handtekening en datum zichtbaar.</t>
-  </si>
-  <si>
     <t>2 Ljubow Popowa - Malerische Architektonik.tif</t>
   </si>
   <si>
@@ -434,12 +299,6 @@
     <t>1 Karl F. Brust - Geheimnisvolles Blau.tif</t>
   </si>
   <si>
-    <t>img_42</t>
-  </si>
-  <si>
-    <t>Het schilderij bestaat uit overlappende geometrische vlakken in aardetinten zoals bruin, zwart, rood en roze. De vormen zijn hoekig en enigszins schuin gerangschikt. De achtergrond is effen, waardoor de gelaagde vlakken worden benadrukt.</t>
-  </si>
-  <si>
     <t>stim_num</t>
   </si>
   <si>
@@ -464,23 +323,14 @@
     <t>stim_type</t>
   </si>
   <si>
-    <t>AI_desc_img</t>
-  </si>
-  <si>
-    <t>description_text</t>
-  </si>
-  <si>
     <t>old_stim_num</t>
-  </si>
-  <si>
-    <t>notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,25 +343,6 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -540,20 +371,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,14 +392,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -616,7 +433,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -722,7 +539,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -864,7 +681,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -872,53 +689,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C69ECA-D0A6-4802-A87B-D6FFC027E7D5}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>134</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
-        <v>135</v>
+        <v>88</v>
       </c>
       <c r="C1" t="s">
-        <v>136</v>
+        <v>89</v>
       </c>
       <c r="D1" t="s">
-        <v>137</v>
+        <v>90</v>
       </c>
       <c r="E1" t="s">
-        <v>138</v>
+        <v>91</v>
       </c>
       <c r="F1" t="s">
-        <v>139</v>
+        <v>92</v>
       </c>
       <c r="G1" t="s">
-        <v>140</v>
+        <v>93</v>
       </c>
       <c r="H1" t="s">
-        <v>141</v>
+        <v>94</v>
       </c>
       <c r="I1" t="s">
-        <v>142</v>
-      </c>
-      <c r="J1" t="s">
-        <v>143</v>
-      </c>
-      <c r="K1" t="s">
-        <v>144</v>
-      </c>
-      <c r="L1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>22</v>
       </c>
@@ -943,17 +751,11 @@
       <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2">
+      <c r="I2">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>23</v>
       </c>
@@ -964,34 +766,25 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3">
+      <c r="I3">
         <v>21</v>
       </c>
-      <c r="L3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>24</v>
       </c>
@@ -1002,31 +795,25 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4">
+        <v>9</v>
+      </c>
+      <c r="I4">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>25</v>
       </c>
@@ -1037,31 +824,25 @@
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>23</v>
+        <v>15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5">
+        <v>9</v>
+      </c>
+      <c r="I5">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>26</v>
       </c>
@@ -1072,34 +853,25 @@
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6">
+      <c r="I6">
         <v>33</v>
       </c>
-      <c r="L6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>27</v>
       </c>
@@ -1110,34 +882,25 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="H7" t="s">
         <v>4</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7">
         <v>38</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="K7">
-        <v>38</v>
-      </c>
-      <c r="L7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>28</v>
       </c>
@@ -1148,34 +911,25 @@
         <v>7</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K8">
+      <c r="I8">
         <v>43</v>
       </c>
-      <c r="L8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>29</v>
       </c>
@@ -1186,34 +940,25 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="H9" t="s">
-        <v>51</v>
-      </c>
-      <c r="I9" t="s">
-        <v>52</v>
-      </c>
-      <c r="J9" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9">
+        <v>34</v>
+      </c>
+      <c r="I9">
         <v>1</v>
       </c>
-      <c r="L9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>30</v>
       </c>
@@ -1224,34 +969,25 @@
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" t="s">
-        <v>59</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="K10">
+        <v>9</v>
+      </c>
+      <c r="I10">
         <v>29</v>
       </c>
-      <c r="L10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>31</v>
       </c>
@@ -1262,31 +998,25 @@
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" t="s">
-        <v>65</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="K11">
+        <v>9</v>
+      </c>
+      <c r="I11">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>32</v>
       </c>
@@ -1297,31 +1027,25 @@
         <v>11</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>69</v>
+        <v>46</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I12" t="s">
-        <v>70</v>
-      </c>
-      <c r="J12" t="s">
-        <v>71</v>
-      </c>
-      <c r="K12">
+      <c r="I12">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>33</v>
       </c>
@@ -1332,34 +1056,25 @@
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="K13">
+        <v>34</v>
+      </c>
+      <c r="I13">
         <v>6</v>
       </c>
-      <c r="L13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>34</v>
       </c>
@@ -1370,34 +1085,25 @@
         <v>13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>79</v>
+        <v>52</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I14" t="s">
-        <v>82</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="K14">
+        <v>34</v>
+      </c>
+      <c r="I14">
         <v>13</v>
       </c>
-      <c r="L14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>35</v>
       </c>
@@ -1408,34 +1114,25 @@
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I15" t="s">
-        <v>89</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="K15">
+        <v>34</v>
+      </c>
+      <c r="I15">
         <v>15</v>
       </c>
-      <c r="L15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>36</v>
       </c>
@@ -1446,34 +1143,25 @@
         <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="H16" t="s">
         <v>4</v>
       </c>
-      <c r="I16" t="s">
-        <v>95</v>
-      </c>
-      <c r="J16" t="s">
-        <v>96</v>
-      </c>
-      <c r="K16">
+      <c r="I16">
         <v>42</v>
       </c>
-      <c r="L16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>37</v>
       </c>
@@ -1484,34 +1172,25 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
       <c r="E17" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
       <c r="F17" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="G17" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="H17" t="s">
-        <v>51</v>
-      </c>
-      <c r="I17" t="s">
-        <v>101</v>
-      </c>
-      <c r="J17" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="K17">
+        <v>34</v>
+      </c>
+      <c r="I17">
         <v>9</v>
       </c>
-      <c r="L17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>38</v>
       </c>
@@ -1522,31 +1201,25 @@
         <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>103</v>
+        <v>67</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>104</v>
+        <v>68</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="K18">
+      <c r="I18">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>39</v>
       </c>
@@ -1557,31 +1230,25 @@
         <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>109</v>
+        <v>71</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>110</v>
+        <v>72</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>111</v>
+        <v>73</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>112</v>
+        <v>74</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I19" t="s">
-        <v>113</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="K19">
+        <v>34</v>
+      </c>
+      <c r="I19">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>40</v>
       </c>
@@ -1592,34 +1259,25 @@
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>115</v>
+        <v>75</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>116</v>
+        <v>76</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I20" t="s">
-        <v>119</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="K20">
+        <v>34</v>
+      </c>
+      <c r="I20">
         <v>12</v>
       </c>
-      <c r="L20" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>41</v>
       </c>
@@ -1630,31 +1288,25 @@
         <v>20</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>123</v>
+        <v>80</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>124</v>
+        <v>81</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>125</v>
+        <v>82</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="K21">
+        <v>9</v>
+      </c>
+      <c r="I21">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>42</v>
       </c>
@@ -1665,27 +1317,21 @@
         <v>21</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>128</v>
+        <v>83</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>129</v>
+        <v>84</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>130</v>
+        <v>85</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>131</v>
+        <v>86</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I22" t="s">
-        <v>132</v>
-      </c>
-      <c r="J22" t="s">
-        <v>133</v>
-      </c>
-      <c r="K22">
+        <v>9</v>
+      </c>
+      <c r="I22">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changing excel file fot round3
</commit_message>
<xml_diff>
--- a/stim_folder/stimuli_round3.xlsx
+++ b/stim_folder/stimuli_round3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amsuni-my.sharepoint.com/personal/a_palmann_uva_nl/Documents/Microsoft Teams Chat Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{F544EB10-FB11-44B7-AA8E-13784B7427AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B95F138F-98EE-4B5C-9BEF-C9A15F666DDC}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="8_{F544EB10-FB11-44B7-AA8E-13784B7427AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C52676F4-E0E6-47B6-97D8-B2B887D4DE94}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5C6A6CE9-FAAA-4323-9214-A09E4F61C974}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{5C6A6CE9-FAAA-4323-9214-A09E4F61C974}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="98">
   <si>
     <t>m_1 Willi Baumeister - Aru mit Gelb.tif</t>
   </si>
@@ -324,6 +324,12 @@
   </si>
   <si>
     <t>old_stim_num</t>
+  </si>
+  <si>
+    <t>target_image</t>
+  </si>
+  <si>
+    <t>simt2</t>
   </si>
 </sst>
 </file>
@@ -390,6 +396,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -689,15 +699,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C69ECA-D0A6-4802-A87B-D6FFC027E7D5}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>87</v>
       </c>
@@ -725,8 +735,11 @@
       <c r="I1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>22</v>
       </c>
@@ -754,8 +767,11 @@
       <c r="I2">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J2" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>23</v>
       </c>
@@ -783,8 +799,11 @@
       <c r="I3">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>24</v>
       </c>
@@ -812,8 +831,11 @@
       <c r="I4">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J4" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>25</v>
       </c>
@@ -841,8 +863,11 @@
       <c r="I5">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>26</v>
       </c>
@@ -870,8 +895,11 @@
       <c r="I6">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J6" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>27</v>
       </c>
@@ -899,8 +927,11 @@
       <c r="I7">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>28</v>
       </c>
@@ -928,8 +959,11 @@
       <c r="I8">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J8" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>29</v>
       </c>
@@ -957,8 +991,11 @@
       <c r="I9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>30</v>
       </c>
@@ -986,8 +1023,11 @@
       <c r="I10">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J10" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>31</v>
       </c>
@@ -1015,8 +1055,11 @@
       <c r="I11">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J11" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>32</v>
       </c>
@@ -1044,8 +1087,11 @@
       <c r="I12">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J12" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>33</v>
       </c>
@@ -1073,8 +1119,11 @@
       <c r="I13">
         <v>6</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J13" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>34</v>
       </c>
@@ -1102,8 +1151,11 @@
       <c r="I14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J14" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>35</v>
       </c>
@@ -1131,8 +1183,11 @@
       <c r="I15">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J15" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>36</v>
       </c>
@@ -1160,8 +1215,11 @@
       <c r="I16">
         <v>42</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J16" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>37</v>
       </c>
@@ -1189,8 +1247,11 @@
       <c r="I17">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J17" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>38</v>
       </c>
@@ -1218,8 +1279,11 @@
       <c r="I18">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J18" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>39</v>
       </c>
@@ -1247,8 +1311,11 @@
       <c r="I19">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J19" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>40</v>
       </c>
@@ -1276,8 +1343,11 @@
       <c r="I20">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J20" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>41</v>
       </c>
@@ -1305,8 +1375,11 @@
       <c r="I21">
         <v>16</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J21" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>42</v>
       </c>
@@ -1333,6 +1406,9 @@
       </c>
       <c r="I22">
         <v>17</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>